<commit_message>
ALTERAÇOES NO BOTÃO DE EDITAR
</commit_message>
<xml_diff>
--- a/teste1912.xlsx
+++ b/teste1912.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BV</t>
+          <t>OC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -539,20 +539,16 @@
       <c r="G2" t="n">
         <v>27</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="H2" t="n">
+        <v>28</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
           <t>DIGITAL</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>123333</t>
-        </is>
+      <c r="J2" t="n">
+        <v>123333</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -609,20 +605,16 @@
       <c r="G3" t="n">
         <v>54785</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>54785</t>
-        </is>
+      <c r="H3" t="n">
+        <v>54785</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>DIGITAL</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>55555</t>
-        </is>
+      <c r="J3" t="n">
+        <v>55555</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -648,17 +640,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Debora Silva</t>
+          <t>GABRIEL PAGOTE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>ITAU</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TESE</t>
+          <t>NOVO</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -668,30 +660,32 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>T490</t>
+          <t>T14</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>AEDSFADEFA</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>45531</v>
+          <t>AESDA</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>555</t>
+        </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>ALLIED</t>
+          <t>55556</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>KKKJ</t>
+          <t>VEFRSS</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>23215614</t>
+          <t>4444</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -701,7 +695,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>5552555</t>
+          <t>44444</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -711,7 +705,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>VENDIDO</t>
+          <t>55555555</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ADICIONADO CAMPO DE PESQUISA
</commit_message>
<xml_diff>
--- a/teste1912.xlsx
+++ b/teste1912.xlsx
@@ -508,7 +508,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GABRIELA</t>
+          <t>GABRIELA PEREIRA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ITAU</t>
+          <t>SANTADER</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -668,25 +668,19 @@
           <t>AESDA</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>555</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>55556</t>
-        </is>
+      <c r="G4" t="n">
+        <v>555</v>
+      </c>
+      <c r="H4" t="n">
+        <v>55556</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
           <t>VEFRSS</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>4444</t>
-        </is>
+      <c r="J4" t="n">
+        <v>4444</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>

</xml_diff>